<commit_message>
feat: complete tuningn/model production
</commit_message>
<xml_diff>
--- a/Output/Model_in_production/Selected_features.xlsx
+++ b/Output/Model_in_production/Selected_features.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>KitchenQual</t>
+          <t>OverallQual</t>
         </is>
       </c>
     </row>
@@ -457,63 +457,63 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>OverallQual</t>
+          <t>FullBath</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ExterQual</t>
+          <t>GarageType_Detchd</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FullBath</t>
+          <t>MSZoning_RM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BsmtQual</t>
+          <t>CentralAir</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FireplaceQu</t>
+          <t>TotalBsmtSF</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GrLivArea</t>
+          <t>Fireplaces</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TotalBsmtSF</t>
+          <t>Neighborhood_Crawfor</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Fireplaces</t>
+          <t>2ndFlrSF</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1stFlrSF</t>
+          <t>GarageType_Attchd</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GarageArea</t>
+          <t>BuildingAge</t>
         </is>
       </c>
     </row>
@@ -541,21 +541,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BuildingAge</t>
+          <t>BsmtExposure_Gd</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TotRmsAbvGrd</t>
+          <t>MSZoning_RL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>KitchenAbvGr</t>
+          <t>SaleType_New</t>
         </is>
       </c>
     </row>
@@ -569,175 +569,294 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HalfBath</t>
+          <t>Neighborhood_OldTown</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2ndFlrSF</t>
+          <t>GarageFinish_Unf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OverallCond</t>
+          <t>Exterior1st_BrkFace</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GarageQual</t>
+          <t>BsmtFinType1_GLQ</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>OpenPorchSF</t>
+          <t>GarageType_No Garage</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BsmtFullBath</t>
+          <t>MasVnrArea</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MasVnrArea</t>
+          <t>OverallCond</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WoodDeckSF</t>
+          <t>GarageQual</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CentralAir</t>
+          <t>ScreenPorch</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LotFrontage</t>
+          <t>HouseStyle_1Story</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GarageCond</t>
+          <t>SaleCondition_Partial</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BedroomAbvGr</t>
+          <t>HouseStyle_2Story</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Fence</t>
+          <t>Foundation_PConc</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BsmtCond</t>
+          <t>RoofMatl_Tar&amp;Grv</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Alley</t>
+          <t>MSZoning_FV</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BsmtUnfSF</t>
+          <t>LotFrontage</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BldgType_TwnhsE</t>
+          <t>OpenPorchSF</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BldgType_Twnhs</t>
+          <t>Neighborhood_NoRidge</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ScreenPorch</t>
+          <t>LotConfig_CulDSac</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BldgType_Duplex</t>
+          <t>RoofStyle_Gambrel</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EnclosedPorch</t>
+          <t>Neighborhood_Timber</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>LowQualFinSF</t>
+          <t>Neighborhood_StoneBr</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BldgType_2fmCon</t>
+          <t>SaleCondition_Normal</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MiscVal</t>
+          <t>BsmtCond</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>3SsnPorch</t>
+          <t>BedroomAbvGr</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>KitchenAbvGr</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SaleType_WD</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Functional_Typ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Exterior1st_CemntBd</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Neighborhood_BrkSide</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>LotShape_Reg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>WoodDeckSF</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Condition1_Norm</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Exterior2nd_VinylSd</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SaleCondition_Family</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Neighborhood_Somerst</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>RoofStyle_Gable</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LandContour_Low</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Neighborhood_NridgHt</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BsmtFinSF2</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Exterior1st_WdShing</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>BsmtHalfBath</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: automate input process
</commit_message>
<xml_diff>
--- a/Output/Model_in_production/Selected_features.xlsx
+++ b/Output/Model_in_production/Selected_features.xlsx
@@ -450,308 +450,308 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GarageCars</t>
+          <t>Foundation_PConc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FullBath</t>
+          <t>Foundation_CBlock</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GarageType_Detchd</t>
+          <t>GarageCars</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MSZoning_RM</t>
+          <t>Fireplaces</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CentralAir</t>
+          <t>TotalBsmtSF</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TotalBsmtSF</t>
+          <t>GarageFinish_Unf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Fireplaces</t>
+          <t>Neighborhood_NridgHt</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Neighborhood_Crawfor</t>
+          <t>MSZoning_RM</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2ndFlrSF</t>
+          <t>BsmtExposure_Gd</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GarageType_Attchd</t>
+          <t>HeatingQC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BsmtFinSF1</t>
+          <t>Neighborhood_NoRidge</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BuildingAge</t>
+          <t>SaleType_New</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HeatingQC</t>
+          <t>GarageFinish_No Garage</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BsmtExposure_Gd</t>
+          <t>BsmtFinType1_GLQ</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MSZoning_RL</t>
+          <t>GarageType_Attchd</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SaleType_New</t>
+          <t>GarageType_BuiltIn</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LotArea</t>
+          <t>SaleCondition_Partial</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Neighborhood_OldTown</t>
+          <t>RoofStyle_Gable</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GarageFinish_Unf</t>
+          <t>BuildingAge</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Exterior1st_BrkFace</t>
+          <t>Exterior2nd_VinylSd</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BsmtFinType1_GLQ</t>
+          <t>Neighborhood_NAmes</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GarageType_No Garage</t>
+          <t>LotArea</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MasVnrArea</t>
+          <t>FullBath</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>OverallCond</t>
+          <t>CentralAir</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GarageQual</t>
+          <t>MSZoning_RL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ScreenPorch</t>
+          <t>MasVnrArea</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>HouseStyle_1Story</t>
+          <t>BsmtExposure_No</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SaleCondition_Partial</t>
+          <t>BsmtFinSF1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HouseStyle_2Story</t>
+          <t>SaleType_WD</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Foundation_PConc</t>
+          <t>Neighborhood_MeadowV</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>RoofMatl_Tar&amp;Grv</t>
+          <t>GarageType_Detchd</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MSZoning_FV</t>
+          <t>OverallCond</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>LotFrontage</t>
+          <t>HouseStyle_2Story</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>OpenPorchSF</t>
+          <t>Exterior1st_BrkFace</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Neighborhood_NoRidge</t>
+          <t>RoofStyle_Hip</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LotConfig_CulDSac</t>
+          <t>LotFrontage</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>RoofStyle_Gambrel</t>
+          <t>BsmtExposure_No Bsmnt</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Neighborhood_Timber</t>
+          <t>Neighborhood_StoneBr</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Neighborhood_StoneBr</t>
+          <t>Neighborhood_Crawfor</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SaleCondition_Normal</t>
+          <t>Exterior1st_CemntBd</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BsmtCond</t>
+          <t>GarageQual</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>BedroomAbvGr</t>
+          <t>GarageType_No Garage</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>KitchenAbvGr</t>
+          <t>2ndFlrSF</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SaleType_WD</t>
+          <t>BsmtCond</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: data input automation
</commit_message>
<xml_diff>
--- a/Output/Model_in_production/Selected_features.xlsx
+++ b/Output/Model_in_production/Selected_features.xlsx
@@ -450,308 +450,308 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Foundation_PConc</t>
+          <t>GarageCars</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Foundation_CBlock</t>
+          <t>FullBath</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GarageCars</t>
+          <t>GarageType_Detchd</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Fireplaces</t>
+          <t>MSZoning_RM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TotalBsmtSF</t>
+          <t>CentralAir</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GarageFinish_Unf</t>
+          <t>TotalBsmtSF</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Neighborhood_NridgHt</t>
+          <t>Fireplaces</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MSZoning_RM</t>
+          <t>Neighborhood_Crawfor</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BsmtExposure_Gd</t>
+          <t>2ndFlrSF</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HeatingQC</t>
+          <t>GarageType_Attchd</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Neighborhood_NoRidge</t>
+          <t>BsmtFinSF1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SaleType_New</t>
+          <t>BuildingAge</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GarageFinish_No Garage</t>
+          <t>HeatingQC</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BsmtFinType1_GLQ</t>
+          <t>BsmtExposure_Gd</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GarageType_Attchd</t>
+          <t>MSZoning_RL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GarageType_BuiltIn</t>
+          <t>SaleType_New</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SaleCondition_Partial</t>
+          <t>LotArea</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RoofStyle_Gable</t>
+          <t>Neighborhood_OldTown</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BuildingAge</t>
+          <t>GarageFinish_Unf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Exterior2nd_VinylSd</t>
+          <t>Exterior1st_BrkFace</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Neighborhood_NAmes</t>
+          <t>BsmtFinType1_GLQ</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LotArea</t>
+          <t>GarageType_No Garage</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>FullBath</t>
+          <t>MasVnrArea</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CentralAir</t>
+          <t>OverallCond</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MSZoning_RL</t>
+          <t>GarageQual</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MasVnrArea</t>
+          <t>ScreenPorch</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BsmtExposure_No</t>
+          <t>HouseStyle_1Story</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BsmtFinSF1</t>
+          <t>SaleCondition_Partial</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SaleType_WD</t>
+          <t>HouseStyle_2Story</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Neighborhood_MeadowV</t>
+          <t>Foundation_PConc</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GarageType_Detchd</t>
+          <t>RoofMatl_Tar&amp;Grv</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>OverallCond</t>
+          <t>MSZoning_FV</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>HouseStyle_2Story</t>
+          <t>LotFrontage</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Exterior1st_BrkFace</t>
+          <t>OpenPorchSF</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>RoofStyle_Hip</t>
+          <t>Neighborhood_NoRidge</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LotFrontage</t>
+          <t>LotConfig_CulDSac</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BsmtExposure_No Bsmnt</t>
+          <t>RoofStyle_Gambrel</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Neighborhood_StoneBr</t>
+          <t>Neighborhood_Timber</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Neighborhood_Crawfor</t>
+          <t>Neighborhood_StoneBr</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Exterior1st_CemntBd</t>
+          <t>SaleCondition_Normal</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GarageQual</t>
+          <t>BsmtCond</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GarageType_No Garage</t>
+          <t>BedroomAbvGr</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2ndFlrSF</t>
+          <t>KitchenAbvGr</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BsmtCond</t>
+          <t>SaleType_WD</t>
         </is>
       </c>
     </row>

</xml_diff>